<commit_message>
Tests and minor improvements
</commit_message>
<xml_diff>
--- a/ExcelHelper/ExcelTables/Частоты.xlsx
+++ b/ExcelHelper/ExcelTables/Частоты.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="клетка" sheetId="1" r:id="rId1"/>
@@ -3818,7 +3818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+    <sheetView topLeftCell="A212" workbookViewId="0">
       <selection activeCell="G229" sqref="G229"/>
     </sheetView>
   </sheetViews>
@@ -19029,7 +19029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added async (IPROGRESS NEEDED)
</commit_message>
<xml_diff>
--- a/ExcelHelper/ExcelTables/Частоты.xlsx
+++ b/ExcelHelper/ExcelTables/Частоты.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="клетка" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="1120">
   <si>
     <t>алгебра</t>
   </si>
@@ -3384,9 +3384,6 @@
   </si>
   <si>
     <t>клетка</t>
-  </si>
-  <si>
-    <t>буба</t>
   </si>
 </sst>
 </file>
@@ -3816,10 +3813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D232"/>
+  <dimension ref="A1:D230"/>
   <sheetViews>
-    <sheetView topLeftCell="A212" workbookViewId="0">
-      <selection activeCell="G229" sqref="G229"/>
+    <sheetView topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="F235" sqref="F235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7041,34 +7038,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B231">
-        <v>1</v>
-      </c>
-      <c r="C231">
-        <v>1</v>
-      </c>
-      <c r="D231">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B232">
-        <v>1</v>
-      </c>
-      <c r="C232">
-        <v>1</v>
-      </c>
-      <c r="D232">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7078,7 +7047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D229"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A208" workbookViewId="0">
       <selection activeCell="D26" sqref="D25:E26"/>
     </sheetView>
   </sheetViews>
@@ -10298,7 +10267,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A190" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -13341,7 +13310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
       <selection activeCell="D1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -15961,7 +15930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D218"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A202" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -19029,7 +18998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A195" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DEMO(excell ex, two tables)
</commit_message>
<xml_diff>
--- a/ExcelHelper/ExcelTables/Частоты.xlsx
+++ b/ExcelHelper/ExcelTables/Частоты.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA008BA3-F4BA-4D3A-B1CC-0C40AC1309D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="клетка" sheetId="1" r:id="rId1"/>
@@ -3389,7 +3390,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3812,10 +3813,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D230"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
       <selection activeCell="F235" sqref="F235"/>
     </sheetView>
   </sheetViews>
@@ -7044,7 +7045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D229"/>
   <sheetViews>
     <sheetView topLeftCell="A208" workbookViewId="0">
@@ -10264,7 +10265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D216"/>
   <sheetViews>
     <sheetView topLeftCell="A190" workbookViewId="0">
@@ -13307,10 +13308,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+    <sheetView topLeftCell="A161" workbookViewId="0">
       <selection activeCell="D1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -15927,7 +15928,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D218"/>
   <sheetViews>
     <sheetView topLeftCell="A202" workbookViewId="0">
@@ -18995,7 +18996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView topLeftCell="A195" workbookViewId="0">

</xml_diff>

<commit_message>
App.config and correct Excel closing
</commit_message>
<xml_diff>
--- a/ExcelHelper/ExcelTables/Частоты.xlsx
+++ b/ExcelHelper/ExcelTables/Частоты.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA008BA3-F4BA-4D3A-B1CC-0C40AC1309D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="клетка" sheetId="1" r:id="rId1"/>
@@ -3390,7 +3389,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3813,7 +3812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D230"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
@@ -7045,7 +7044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D229"/>
   <sheetViews>
     <sheetView topLeftCell="A208" workbookViewId="0">
@@ -10265,7 +10264,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D216"/>
   <sheetViews>
     <sheetView topLeftCell="A190" workbookViewId="0">
@@ -13308,7 +13307,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D186"/>
   <sheetViews>
     <sheetView topLeftCell="A161" workbookViewId="0">
@@ -15928,7 +15927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D218"/>
   <sheetViews>
     <sheetView topLeftCell="A202" workbookViewId="0">
@@ -18996,7 +18995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView topLeftCell="A195" workbookViewId="0">

</xml_diff>